<commit_message>
Update comparison - 10 runs for last query
</commit_message>
<xml_diff>
--- a/notebook/comparison.xlsx
+++ b/notebook/comparison.xlsx
@@ -133,9 +133,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -158,10 +162,10 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
+      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.41"/>
@@ -489,8 +493,39 @@
       <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>201536</v>
+      <c r="B10" s="1" t="n">
+        <v>185620</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>184710</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>185580</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>182315</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>183207</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>183886</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>181302</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>181158</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>182356</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>183611</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">AVERAGE(B10:K10)</f>
+        <v>183374.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Rename queries, update notebbok
</commit_message>
<xml_diff>
--- a/notebook/comparison.xlsx
+++ b/notebook/comparison.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t xml:space="preserve">OntopSpark</t>
   </si>
   <si>
+    <t xml:space="preserve">AVERAGE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q1</t>
   </si>
   <si>
@@ -46,10 +49,10 @@
     <t xml:space="preserve">Q8</t>
   </si>
   <si>
-    <t xml:space="preserve">FREE_SUBJ_PRED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENTAILMENT</t>
+    <t xml:space="preserve">Q(?s ?p)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q(?s ?p ?o)</t>
   </si>
   <si>
     <t xml:space="preserve">SANSA</t>
@@ -68,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -89,6 +92,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,9 +143,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -162,10 +176,10 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.41"/>
@@ -176,10 +190,13 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>3560</v>
@@ -218,7 +235,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3094</v>
@@ -257,7 +274,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1326</v>
@@ -296,7 +313,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1985</v>
@@ -335,7 +352,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1574</v>
@@ -374,7 +391,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1893</v>
@@ -413,7 +430,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2105</v>
@@ -452,7 +469,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>14455</v>
@@ -491,36 +508,36 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>185620</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>184710</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="2" t="n">
         <v>185580</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>182315</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="2" t="n">
         <v>183207</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="2" t="n">
         <v>183886</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="2" t="n">
         <v>181302</v>
       </c>
-      <c r="I10" s="1" t="n">
+      <c r="I10" s="2" t="n">
         <v>181158</v>
       </c>
-      <c r="J10" s="1" t="n">
+      <c r="J10" s="2" t="n">
         <v>182356</v>
       </c>
-      <c r="K10" s="1" t="n">
+      <c r="K10" s="2" t="n">
         <v>183611</v>
       </c>
       <c r="M10" s="0" t="n">
@@ -530,12 +547,12 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>3054</v>
@@ -574,7 +591,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1046</v>
@@ -613,7 +630,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1050</v>
@@ -652,7 +669,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2064</v>
@@ -691,7 +708,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1464</v>
@@ -730,7 +747,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1319</v>
@@ -769,7 +786,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1788</v>
@@ -808,7 +825,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>2821</v>
@@ -847,7 +864,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1782</v>

</xml_diff>